<commit_message>
new value of game
</commit_message>
<xml_diff>
--- a/excelToJson/Value.xlsx
+++ b/excelToJson/Value.xlsx
@@ -47,6 +47,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b val="true"/>
@@ -54,6 +55,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -576,7 +578,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1713</v>
+        <v>1800</v>
       </c>
       <c r="C6" s="1">
         <v>82</v>
@@ -605,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1839</v>
+        <v>1338</v>
       </c>
       <c r="C7" s="1">
         <v>84</v>
@@ -634,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1944</v>
+        <v>1806</v>
       </c>
       <c r="C8" s="1">
         <v>86</v>
@@ -663,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>4071</v>
+        <v>2507</v>
       </c>
       <c r="C9" s="1">
         <v>160</v>
@@ -692,7 +694,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>4230</v>
+        <v>2995</v>
       </c>
       <c r="C10" s="1">
         <v>162</v>
@@ -721,7 +723,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>4372</v>
+        <v>4616</v>
       </c>
       <c r="C11" s="1">
         <v>164</v>
@@ -740,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4616</v>
+        <v>4740</v>
       </c>
       <c r="C12" s="1">
         <v>166</v>
@@ -759,7 +761,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4821</v>
+        <v>4853</v>
       </c>
       <c r="C13" s="1">
         <v>168</v>
@@ -778,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>9970</v>
+        <v>5931</v>
       </c>
       <c r="C14" s="1">
         <v>313</v>
@@ -797,7 +799,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>10281</v>
+        <v>6047</v>
       </c>
       <c r="C15" s="1">
         <v>315</v>
@@ -816,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>10559</v>
+        <v>10377</v>
       </c>
       <c r="C16" s="1">
         <v>317</v>
@@ -835,7 +837,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>10810</v>
+        <v>9503</v>
       </c>
       <c r="C17" s="1">
         <v>319</v>
@@ -854,7 +856,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>11038</v>
+        <v>10729</v>
       </c>
       <c r="C18" s="1">
         <v>321</v>
@@ -873,7 +875,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>11248</v>
+        <v>10888</v>
       </c>
       <c r="C19" s="1">
         <v>323</v>
@@ -892,7 +894,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>11443</v>
+        <v>11145</v>
       </c>
       <c r="C20" s="1">
         <v>325</v>
@@ -911,7 +913,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>11623</v>
+        <v>11504</v>
       </c>
       <c r="C21" s="1">
         <v>327</v>
@@ -926,804 +928,1524 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>11609</v>
+      </c>
+      <c r="C22" s="1">
+        <v>329</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
+      <c r="I22" s="1">
+        <v>134143</v>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>14032</v>
+      </c>
+      <c r="C23" s="1">
+        <v>617</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
+      <c r="I23" s="1">
+        <v>178544</v>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1">
+        <v>21222</v>
+      </c>
+      <c r="C24" s="1">
+        <v>619</v>
+      </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
+      <c r="I24" s="1">
+        <v>237643</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1">
+        <v>23766</v>
+      </c>
+      <c r="C25" s="1">
+        <v>621</v>
+      </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
+      <c r="I25" s="1">
+        <v>316302</v>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1">
+        <v>28943</v>
+      </c>
+      <c r="C26" s="1">
+        <v>623</v>
+      </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
+      <c r="I26" s="1">
+        <v>420998</v>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1">
+        <v>24311</v>
+      </c>
+      <c r="C27" s="1">
+        <v>625</v>
+      </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
+      <c r="I27" s="1">
+        <v>560348</v>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1">
+        <v>26945</v>
+      </c>
+      <c r="C28" s="1">
+        <v>627</v>
+      </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
+      <c r="I28" s="1">
+        <v>745823</v>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1">
+        <v>29609</v>
+      </c>
+      <c r="C29" s="1">
+        <v>629</v>
+      </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
+      <c r="I29" s="1">
+        <v>992690</v>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1">
+        <v>32300</v>
+      </c>
+      <c r="C30" s="1">
+        <v>631</v>
+      </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
+      <c r="I30" s="1">
+        <v>1321271</v>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1">
+        <v>40592</v>
+      </c>
+      <c r="C31" s="1">
+        <v>633</v>
+      </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
+      <c r="I31" s="1">
+        <v>1758611</v>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1">
+        <v>35677</v>
+      </c>
+      <c r="C32" s="1">
+        <v>635</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
+      <c r="I32" s="1">
+        <v>2340711</v>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1">
+        <v>35833</v>
+      </c>
+      <c r="C33" s="1">
+        <v>637</v>
+      </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
+      <c r="I33" s="1">
+        <v>3115486</v>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1">
+        <v>35985</v>
+      </c>
+      <c r="C34" s="1">
+        <v>639</v>
+      </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
+      <c r="I34" s="1">
+        <v>4146712</v>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1">
+        <v>36135</v>
+      </c>
+      <c r="C35" s="1">
+        <v>641</v>
+      </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
+      <c r="I35" s="1">
+        <v>5519274</v>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>36377</v>
+      </c>
+      <c r="C36" s="1">
+        <v>643</v>
+      </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
+      <c r="I36" s="1">
+        <v>7346153</v>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1">
+        <v>26101</v>
+      </c>
+      <c r="C37" s="1">
+        <v>645</v>
+      </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
+      <c r="I37" s="1">
+        <v>9777729</v>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1">
+        <v>26216</v>
+      </c>
+      <c r="C38" s="1">
+        <v>647</v>
+      </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
+      <c r="I38" s="1">
+        <v>13014158</v>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1">
+        <v>26329</v>
+      </c>
+      <c r="C39" s="1">
+        <v>649</v>
+      </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
+      <c r="I39" s="1">
+        <v>17321844</v>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1">
+        <v>26439</v>
+      </c>
+      <c r="C40" s="1">
+        <v>651</v>
+      </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
+      <c r="I40" s="1">
+        <v>23055374</v>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1">
+        <v>42834</v>
+      </c>
+      <c r="C41" s="1">
+        <v>653</v>
+      </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
+      <c r="I41" s="1">
+        <v>30686702</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1">
+        <v>26858</v>
+      </c>
+      <c r="C42" s="1">
+        <v>655</v>
+      </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
+      <c r="I42" s="1">
+        <v>40844001</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1">
+        <v>28021</v>
+      </c>
+      <c r="C43" s="1">
+        <v>1231</v>
+      </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
+      <c r="I43" s="1">
+        <v>54363365</v>
+      </c>
     </row>
     <row r="44">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1">
+        <v>32433</v>
+      </c>
+      <c r="C44" s="1">
+        <v>1233</v>
+      </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
+      <c r="I44" s="1">
+        <v>72357638</v>
+      </c>
     </row>
     <row r="45">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1">
+        <v>37954</v>
+      </c>
+      <c r="C45" s="1">
+        <v>1235</v>
+      </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
+      <c r="I45" s="1">
+        <v>96308016</v>
+      </c>
     </row>
     <row r="46">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1">
+        <v>54384</v>
+      </c>
+      <c r="C46" s="1">
+        <v>1237</v>
+      </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
+      <c r="I46" s="1">
+        <v>128185969</v>
+      </c>
     </row>
     <row r="47">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1">
+        <v>54597</v>
+      </c>
+      <c r="C47" s="1">
+        <v>1239</v>
+      </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
+      <c r="I47" s="1">
+        <v>170615525</v>
+      </c>
     </row>
     <row r="48">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1">
+        <v>54806</v>
+      </c>
+      <c r="C48" s="1">
+        <v>1241</v>
+      </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
+      <c r="I48" s="1">
+        <v>227089264</v>
+      </c>
     </row>
     <row r="49">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1">
+        <v>55011</v>
+      </c>
+      <c r="C49" s="1">
+        <v>1243</v>
+      </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
+      <c r="I49" s="1">
+        <v>302255810</v>
+      </c>
     </row>
     <row r="50">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="1">
+        <v>55212</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1245</v>
+      </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
+      <c r="I50" s="1">
+        <v>402302483</v>
+      </c>
     </row>
     <row r="51">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="1">
+        <v>66491</v>
+      </c>
+      <c r="C51" s="1">
+        <v>1247</v>
+      </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
+      <c r="I51" s="1">
+        <v>535464604</v>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="1">
+        <v>55554</v>
+      </c>
+      <c r="C52" s="1">
+        <v>1249</v>
+      </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
+      <c r="I52" s="1">
+        <v>712703388</v>
+      </c>
     </row>
     <row r="53">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="1">
+        <v>55697</v>
+      </c>
+      <c r="C53" s="1">
+        <v>1251</v>
+      </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
+      <c r="I53" s="1">
+        <v>948608209</v>
+      </c>
     </row>
     <row r="54">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="1">
+        <v>55839</v>
+      </c>
+      <c r="C54" s="1">
+        <v>1253</v>
+      </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
+      <c r="I54" s="1">
+        <v>1262597526</v>
+      </c>
     </row>
     <row r="55">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="1">
+        <v>55978</v>
+      </c>
+      <c r="C55" s="1">
+        <v>1255</v>
+      </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
+      <c r="I55" s="1">
+        <v>1680517307</v>
+      </c>
     </row>
     <row r="56">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="1">
+        <v>67339</v>
+      </c>
+      <c r="C56" s="1">
+        <v>1257</v>
+      </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
+      <c r="I56" s="1">
+        <v>2236768536</v>
+      </c>
     </row>
     <row r="57">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="1">
+        <v>56274</v>
+      </c>
+      <c r="C57" s="1">
+        <v>1259</v>
+      </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
+      <c r="I57" s="1">
+        <v>2977138921</v>
+      </c>
     </row>
     <row r="58">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="1">
+        <v>56430</v>
+      </c>
+      <c r="C58" s="1">
+        <v>1261</v>
+      </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
+      <c r="I58" s="1">
+        <v>3962571904</v>
+      </c>
     </row>
     <row r="59">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="1">
+        <v>56584</v>
+      </c>
+      <c r="C59" s="1">
+        <v>1263</v>
+      </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
+      <c r="I59" s="1">
+        <v>5274183204</v>
+      </c>
     </row>
     <row r="60">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="1">
+        <v>56735</v>
+      </c>
+      <c r="C60" s="1">
+        <v>1265</v>
+      </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
+      <c r="I60" s="1">
+        <v>7019937844</v>
+      </c>
     </row>
     <row r="61">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="1">
+        <v>74356</v>
+      </c>
+      <c r="C61" s="1">
+        <v>1267</v>
+      </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
+      <c r="I61" s="1">
+        <v>9343537270</v>
+      </c>
     </row>
     <row r="62">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="1">
+        <v>57339</v>
+      </c>
+      <c r="C62" s="1">
+        <v>1269</v>
+      </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
+      <c r="I62" s="1">
+        <v>12436248106</v>
+      </c>
     </row>
     <row r="63">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="1">
+        <v>57480</v>
+      </c>
+      <c r="C63" s="1">
+        <v>1271</v>
+      </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
+      <c r="I63" s="1">
+        <v>16552646230</v>
+      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="1">
+        <v>57619</v>
+      </c>
+      <c r="C64" s="1">
+        <v>1273</v>
+      </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
+      <c r="I64" s="1">
+        <v>22031572131</v>
+      </c>
     </row>
     <row r="65">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="1">
+        <v>57756</v>
+      </c>
+      <c r="C65" s="1">
+        <v>1275</v>
+      </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
+      <c r="I65" s="1">
+        <v>29324022507</v>
+      </c>
     </row>
     <row r="66">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="1">
+        <v>69469</v>
+      </c>
+      <c r="C66" s="1">
+        <v>1277</v>
+      </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
+      <c r="I66" s="1">
+        <v>39030273956</v>
+      </c>
     </row>
     <row r="67">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1"/>
-      <c r="C67" s="1"/>
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="1">
+        <v>58043</v>
+      </c>
+      <c r="C67" s="1">
+        <v>1279</v>
+      </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
+      <c r="I67" s="1">
+        <v>51949294636</v>
+      </c>
     </row>
     <row r="68">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1"/>
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="1">
+        <v>58194</v>
+      </c>
+      <c r="C68" s="1">
+        <v>1281</v>
+      </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
+      <c r="I68" s="1">
+        <v>69144511160</v>
+      </c>
     </row>
     <row r="69">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="1"/>
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="1">
+        <v>58342</v>
+      </c>
+      <c r="C69" s="1">
+        <v>1283</v>
+      </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
+      <c r="I69" s="1">
+        <v>92031344353</v>
+      </c>
     </row>
     <row r="70">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="1">
+        <v>58488</v>
+      </c>
+      <c r="C70" s="1">
+        <v>1285</v>
+      </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
+      <c r="I70" s="1">
+        <v>122493719334</v>
+      </c>
     </row>
     <row r="71">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1">
+        <v>82258</v>
+      </c>
+      <c r="C71" s="1">
+        <v>1287</v>
+      </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
+      <c r="I71" s="1">
+        <v>163039140434</v>
+      </c>
     </row>
     <row r="72">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="1">
+        <v>58896</v>
+      </c>
+      <c r="C72" s="1">
+        <v>1289</v>
+      </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
+      <c r="I72" s="1">
+        <v>217005095917</v>
+      </c>
     </row>
     <row r="73">
-      <c r="A73" s="1"/>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="1">
+        <v>59035</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1291</v>
+      </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
+      <c r="I73" s="1">
+        <v>288833782666</v>
+      </c>
     </row>
     <row r="74">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1"/>
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="1">
+        <v>59171</v>
+      </c>
+      <c r="C74" s="1">
+        <v>1293</v>
+      </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
+      <c r="I74" s="1">
+        <v>384437764728</v>
+      </c>
     </row>
     <row r="75">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1"/>
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="1">
+        <v>59306</v>
+      </c>
+      <c r="C75" s="1">
+        <v>1295</v>
+      </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
+      <c r="I75" s="1">
+        <v>511686664853</v>
+      </c>
     </row>
     <row r="76">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1"/>
-      <c r="C76" s="1"/>
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="1">
+        <v>77271</v>
+      </c>
+      <c r="C76" s="1">
+        <v>1297</v>
+      </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
+      <c r="I76" s="1">
+        <v>681054950919</v>
+      </c>
     </row>
     <row r="77">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="1"/>
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="1">
+        <v>59603</v>
+      </c>
+      <c r="C77" s="1">
+        <v>1299</v>
+      </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
+      <c r="I77" s="1">
+        <v>906484139672</v>
+      </c>
     </row>
     <row r="78">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="1">
+        <v>59764</v>
+      </c>
+      <c r="C78" s="1">
+        <v>1301</v>
+      </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
+      <c r="I78" s="1">
+        <v>1206530389904</v>
+      </c>
     </row>
     <row r="79">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1"/>
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="1">
+        <v>59923</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1303</v>
+      </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
+      <c r="I79" s="1">
+        <v>1605891948962</v>
+      </c>
     </row>
     <row r="80">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="1">
+        <v>60080</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1305</v>
+      </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
+      <c r="I80" s="1">
+        <v>2137442184068</v>
+      </c>
     </row>
     <row r="81">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="1">
+        <v>84413</v>
+      </c>
+      <c r="C81" s="1">
+        <v>1307</v>
+      </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
+      <c r="I81" s="1">
+        <v>2844935546994</v>
+      </c>
     </row>
     <row r="82">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="1">
+        <v>60401</v>
+      </c>
+      <c r="C82" s="1">
+        <v>1309</v>
+      </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
+      <c r="I82" s="1">
+        <v>3786609213049</v>
+      </c>
     </row>
     <row r="83">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="1">
+        <v>60506</v>
+      </c>
+      <c r="C83" s="1">
+        <v>1311</v>
+      </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
+      <c r="I83" s="1">
+        <v>5039976862569</v>
+      </c>
     </row>
     <row r="84">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="1">
+        <v>60609</v>
+      </c>
+      <c r="C84" s="1">
+        <v>1313</v>
+      </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
+      <c r="I84" s="1">
+        <v>6708209204079</v>
+      </c>
     </row>
     <row r="85">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1">
+        <v>60712</v>
+      </c>
+      <c r="C85" s="1">
+        <v>1315</v>
+      </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
+      <c r="I85" s="1">
+        <v>8928626450629</v>
+      </c>
     </row>
     <row r="86">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1">
+        <v>97555</v>
+      </c>
+      <c r="C86" s="1">
+        <v>2464</v>
+      </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
+      <c r="I86" s="1">
+        <v>11884001805786</v>
+      </c>
     </row>
     <row r="87">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="1">
+        <v>83076</v>
+      </c>
+      <c r="C87" s="1">
+        <v>2466</v>
+      </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
+      <c r="I87" s="1">
+        <v>15817606403502</v>
+      </c>
     </row>
     <row r="88">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="1"/>
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="1">
+        <v>97916</v>
+      </c>
+      <c r="C88" s="1">
+        <v>2468</v>
+      </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
+      <c r="I88" s="1">
+        <v>21053234123061</v>
+      </c>
     </row>
     <row r="89">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="1">
+        <v>122617</v>
+      </c>
+      <c r="C89" s="1">
+        <v>2470</v>
+      </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
+      <c r="I89" s="1">
+        <v>28021854617793</v>
+      </c>
     </row>
     <row r="90">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="1">
+        <v>122837</v>
+      </c>
+      <c r="C90" s="1">
+        <v>2472</v>
+      </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
+      <c r="I90" s="1">
+        <v>37297088496283</v>
+      </c>
     </row>
     <row r="91">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="1">
+        <v>147923</v>
+      </c>
+      <c r="C91" s="1">
+        <v>2474</v>
+      </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
+      <c r="I91" s="1">
+        <v>49642424788552</v>
+      </c>
     </row>
     <row r="92">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="1">
+        <v>123482</v>
+      </c>
+      <c r="C92" s="1">
+        <v>2476</v>
+      </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
+      <c r="I92" s="1">
+        <v>66074067393563</v>
+      </c>
     </row>
     <row r="93">
-      <c r="A93" s="1"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="1">
+        <v>136061</v>
+      </c>
+      <c r="C93" s="1">
+        <v>2478</v>
+      </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
+      <c r="I93" s="1">
+        <v>87944583700832</v>
+      </c>
     </row>
     <row r="94">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="1">
+        <v>142486</v>
+      </c>
+      <c r="C94" s="1">
+        <v>2480</v>
+      </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
+      <c r="I94" s="1">
+        <v>117054240905808</v>
+      </c>
     </row>
     <row r="95">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="1">
+        <v>148928</v>
+      </c>
+      <c r="C95" s="1">
+        <v>2482</v>
+      </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
+      <c r="I95" s="1">
+        <v>155799194645630</v>
+      </c>
     </row>
     <row r="96">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="1">
+        <v>166916</v>
+      </c>
+      <c r="C96" s="1">
+        <v>2484</v>
+      </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
+      <c r="I96" s="1">
+        <v>207368728073333</v>
+      </c>
     </row>
     <row r="97">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="1">
+        <v>124764</v>
+      </c>
+      <c r="C97" s="1">
+        <v>2486</v>
+      </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
+      <c r="I97" s="1">
+        <v>276007777065606</v>
+      </c>
     </row>
     <row r="98">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1">
+        <v>124962</v>
+      </c>
+      <c r="C98" s="1">
+        <v>2488</v>
+      </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
+      <c r="I98" s="1">
+        <v>367366351274322</v>
+      </c>
     </row>
     <row r="99">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1">
+        <v>125158</v>
+      </c>
+      <c r="C99" s="1">
+        <v>2490</v>
+      </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
+      <c r="I99" s="1">
+        <v>488964613546122</v>
+      </c>
     </row>
     <row r="100">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1">
+        <v>125352</v>
+      </c>
+      <c r="C100" s="1">
+        <v>2492</v>
+      </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
+      <c r="I100" s="1">
+        <v>650811900629889</v>
+      </c>
     </row>
     <row r="101">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1">
+        <v>200872</v>
+      </c>
+      <c r="C101" s="1">
+        <v>2494</v>
+      </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
+      <c r="I101" s="1">
+        <v>866230639738382</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="1"/>
@@ -1734,6 +2456,7 @@
       <c r="F102" s="1"/>
       <c r="G102" s="1"/>
       <c r="H102" s="1"/>
+      <c r="I102" s="1"/>
     </row>
     <row r="103">
       <c r="A103" s="1"/>
@@ -1744,6 +2467,7 @@
       <c r="F103" s="1"/>
       <c r="G103" s="1"/>
       <c r="H103" s="1"/>
+      <c r="I103" s="1"/>
     </row>
     <row r="104">
       <c r="A104" s="1"/>
@@ -1754,6 +2478,7 @@
       <c r="F104" s="1"/>
       <c r="G104" s="1"/>
       <c r="H104" s="1"/>
+      <c r="I104" s="1"/>
     </row>
     <row r="105">
       <c r="A105" s="1"/>
@@ -1764,6 +2489,7 @@
       <c r="F105" s="1"/>
       <c r="G105" s="1"/>
       <c r="H105" s="1"/>
+      <c r="I105" s="1"/>
     </row>
     <row r="106">
       <c r="A106" s="1"/>
@@ -1774,6 +2500,7 @@
       <c r="F106" s="1"/>
       <c r="G106" s="1"/>
       <c r="H106" s="1"/>
+      <c r="I106" s="1"/>
     </row>
     <row r="107">
       <c r="A107" s="1"/>
@@ -1784,6 +2511,7 @@
       <c r="F107" s="1"/>
       <c r="G107" s="1"/>
       <c r="H107" s="1"/>
+      <c r="I107" s="1"/>
     </row>
     <row r="108">
       <c r="A108" s="1"/>
@@ -1794,6 +2522,7 @@
       <c r="F108" s="1"/>
       <c r="G108" s="1"/>
       <c r="H108" s="1"/>
+      <c r="I108" s="1"/>
     </row>
     <row r="109">
       <c r="A109" s="1"/>
@@ -1804,6 +2533,7 @@
       <c r="F109" s="1"/>
       <c r="G109" s="1"/>
       <c r="H109" s="1"/>
+      <c r="I109" s="1"/>
     </row>
     <row r="110">
       <c r="A110" s="1"/>
@@ -1814,6 +2544,7 @@
       <c r="F110" s="1"/>
       <c r="G110" s="1"/>
       <c r="H110" s="1"/>
+      <c r="I110" s="1"/>
     </row>
     <row r="111">
       <c r="A111" s="1"/>
@@ -1824,6 +2555,7 @@
       <c r="F111" s="1"/>
       <c r="G111" s="1"/>
       <c r="H111" s="1"/>
+      <c r="I111" s="1"/>
     </row>
     <row r="112">
       <c r="A112" s="1"/>
@@ -1834,6 +2566,7 @@
       <c r="F112" s="1"/>
       <c r="G112" s="1"/>
       <c r="H112" s="1"/>
+      <c r="I112" s="1"/>
     </row>
     <row r="113">
       <c r="A113" s="1"/>
@@ -1844,6 +2577,7 @@
       <c r="F113" s="1"/>
       <c r="G113" s="1"/>
       <c r="H113" s="1"/>
+      <c r="I113" s="1"/>
     </row>
     <row r="114">
       <c r="A114" s="1"/>
@@ -1854,6 +2588,7 @@
       <c r="F114" s="1"/>
       <c r="G114" s="1"/>
       <c r="H114" s="1"/>
+      <c r="I114" s="1"/>
     </row>
     <row r="115">
       <c r="A115" s="1"/>
@@ -1864,6 +2599,7 @@
       <c r="F115" s="1"/>
       <c r="G115" s="1"/>
       <c r="H115" s="1"/>
+      <c r="I115" s="1"/>
     </row>
     <row r="116">
       <c r="A116" s="1"/>
@@ -1874,6 +2610,7 @@
       <c r="F116" s="1"/>
       <c r="G116" s="1"/>
       <c r="H116" s="1"/>
+      <c r="I116" s="1"/>
     </row>
     <row r="117">
       <c r="A117" s="1"/>
@@ -1884,6 +2621,7 @@
       <c r="F117" s="1"/>
       <c r="G117" s="1"/>
       <c r="H117" s="1"/>
+      <c r="I117" s="1"/>
     </row>
     <row r="118">
       <c r="A118" s="1"/>
@@ -1894,6 +2632,7 @@
       <c r="F118" s="1"/>
       <c r="G118" s="1"/>
       <c r="H118" s="1"/>
+      <c r="I118" s="1"/>
     </row>
     <row r="119">
       <c r="A119" s="1"/>
@@ -1904,6 +2643,7 @@
       <c r="F119" s="1"/>
       <c r="G119" s="1"/>
       <c r="H119" s="1"/>
+      <c r="I119" s="1"/>
     </row>
     <row r="120">
       <c r="A120" s="1"/>
@@ -1914,6 +2654,7 @@
       <c r="F120" s="1"/>
       <c r="G120" s="1"/>
       <c r="H120" s="1"/>
+      <c r="I120" s="1"/>
     </row>
     <row r="121">
       <c r="A121" s="1"/>
@@ -1924,6 +2665,7 @@
       <c r="F121" s="1"/>
       <c r="G121" s="1"/>
       <c r="H121" s="1"/>
+      <c r="I121" s="1"/>
     </row>
     <row r="122">
       <c r="A122" s="1"/>
@@ -1934,6 +2676,7 @@
       <c r="F122" s="1"/>
       <c r="G122" s="1"/>
       <c r="H122" s="1"/>
+      <c r="I122" s="1"/>
     </row>
     <row r="123">
       <c r="A123" s="1"/>
@@ -1944,6 +2687,7 @@
       <c r="F123" s="1"/>
       <c r="G123" s="1"/>
       <c r="H123" s="1"/>
+      <c r="I123" s="1"/>
     </row>
     <row r="124">
       <c r="A124" s="1"/>
@@ -1954,6 +2698,7 @@
       <c r="F124" s="1"/>
       <c r="G124" s="1"/>
       <c r="H124" s="1"/>
+      <c r="I124" s="1"/>
     </row>
     <row r="125">
       <c r="A125" s="1"/>
@@ -1964,6 +2709,7 @@
       <c r="F125" s="1"/>
       <c r="G125" s="1"/>
       <c r="H125" s="1"/>
+      <c r="I125" s="1"/>
     </row>
     <row r="126">
       <c r="A126" s="1"/>
@@ -1974,6 +2720,7 @@
       <c r="F126" s="1"/>
       <c r="G126" s="1"/>
       <c r="H126" s="1"/>
+      <c r="I126" s="1"/>
     </row>
     <row r="127">
       <c r="A127" s="1"/>
@@ -1984,6 +2731,7 @@
       <c r="F127" s="1"/>
       <c r="G127" s="1"/>
       <c r="H127" s="1"/>
+      <c r="I127" s="1"/>
     </row>
     <row r="128">
       <c r="A128" s="1"/>
@@ -1994,6 +2742,7 @@
       <c r="F128" s="1"/>
       <c r="G128" s="1"/>
       <c r="H128" s="1"/>
+      <c r="I128" s="1"/>
     </row>
     <row r="129">
       <c r="A129" s="1"/>
@@ -2004,6 +2753,7 @@
       <c r="F129" s="1"/>
       <c r="G129" s="1"/>
       <c r="H129" s="1"/>
+      <c r="I129" s="1"/>
     </row>
     <row r="130">
       <c r="A130" s="1"/>
@@ -2014,6 +2764,7 @@
       <c r="F130" s="1"/>
       <c r="G130" s="1"/>
       <c r="H130" s="1"/>
+      <c r="I130" s="1"/>
     </row>
     <row r="131">
       <c r="A131" s="1"/>
@@ -2024,6 +2775,7 @@
       <c r="F131" s="1"/>
       <c r="G131" s="1"/>
       <c r="H131" s="1"/>
+      <c r="I131" s="1"/>
     </row>
     <row r="132">
       <c r="A132" s="1"/>
@@ -2034,6 +2786,7 @@
       <c r="F132" s="1"/>
       <c r="G132" s="1"/>
       <c r="H132" s="1"/>
+      <c r="I132" s="1"/>
     </row>
     <row r="133">
       <c r="A133" s="1"/>
@@ -2044,6 +2797,7 @@
       <c r="F133" s="1"/>
       <c r="G133" s="1"/>
       <c r="H133" s="1"/>
+      <c r="I133" s="1"/>
     </row>
     <row r="134">
       <c r="A134" s="1"/>
@@ -2054,6 +2808,7 @@
       <c r="F134" s="1"/>
       <c r="G134" s="1"/>
       <c r="H134" s="1"/>
+      <c r="I134" s="1"/>
     </row>
     <row r="135">
       <c r="A135" s="1"/>
@@ -2064,6 +2819,7 @@
       <c r="F135" s="1"/>
       <c r="G135" s="1"/>
       <c r="H135" s="1"/>
+      <c r="I135" s="1"/>
     </row>
     <row r="136">
       <c r="A136" s="1"/>
@@ -2074,6 +2830,7 @@
       <c r="F136" s="1"/>
       <c r="G136" s="1"/>
       <c r="H136" s="1"/>
+      <c r="I136" s="1"/>
     </row>
     <row r="137">
       <c r="A137" s="1"/>
@@ -2084,6 +2841,7 @@
       <c r="F137" s="1"/>
       <c r="G137" s="1"/>
       <c r="H137" s="1"/>
+      <c r="I137" s="1"/>
     </row>
     <row r="138">
       <c r="A138" s="1"/>
@@ -2094,6 +2852,7 @@
       <c r="F138" s="1"/>
       <c r="G138" s="1"/>
       <c r="H138" s="1"/>
+      <c r="I138" s="1"/>
     </row>
     <row r="139">
       <c r="A139" s="1"/>
@@ -2104,6 +2863,7 @@
       <c r="F139" s="1"/>
       <c r="G139" s="1"/>
       <c r="H139" s="1"/>
+      <c r="I139" s="1"/>
     </row>
     <row r="140">
       <c r="A140" s="1"/>
@@ -2114,6 +2874,7 @@
       <c r="F140" s="1"/>
       <c r="G140" s="1"/>
       <c r="H140" s="1"/>
+      <c r="I140" s="1"/>
     </row>
     <row r="141">
       <c r="A141" s="1"/>
@@ -2124,6 +2885,7 @@
       <c r="F141" s="1"/>
       <c r="G141" s="1"/>
       <c r="H141" s="1"/>
+      <c r="I141" s="1"/>
     </row>
     <row r="142">
       <c r="A142" s="1"/>
@@ -2134,6 +2896,7 @@
       <c r="F142" s="1"/>
       <c r="G142" s="1"/>
       <c r="H142" s="1"/>
+      <c r="I142" s="1"/>
     </row>
     <row r="143">
       <c r="A143" s="1"/>
@@ -2144,6 +2907,7 @@
       <c r="F143" s="1"/>
       <c r="G143" s="1"/>
       <c r="H143" s="1"/>
+      <c r="I143" s="1"/>
     </row>
     <row r="144">
       <c r="A144" s="1"/>
@@ -2154,6 +2918,7 @@
       <c r="F144" s="1"/>
       <c r="G144" s="1"/>
       <c r="H144" s="1"/>
+      <c r="I144" s="1"/>
     </row>
     <row r="145">
       <c r="A145" s="1"/>
@@ -2164,6 +2929,7 @@
       <c r="F145" s="1"/>
       <c r="G145" s="1"/>
       <c r="H145" s="1"/>
+      <c r="I145" s="1"/>
     </row>
     <row r="146">
       <c r="A146" s="1"/>
@@ -2174,6 +2940,7 @@
       <c r="F146" s="1"/>
       <c r="G146" s="1"/>
       <c r="H146" s="1"/>
+      <c r="I146" s="1"/>
     </row>
     <row r="147">
       <c r="A147" s="1"/>
@@ -2184,6 +2951,7 @@
       <c r="F147" s="1"/>
       <c r="G147" s="1"/>
       <c r="H147" s="1"/>
+      <c r="I147" s="1"/>
     </row>
     <row r="148">
       <c r="A148" s="1"/>
@@ -2194,6 +2962,7 @@
       <c r="F148" s="1"/>
       <c r="G148" s="1"/>
       <c r="H148" s="1"/>
+      <c r="I148" s="1"/>
     </row>
     <row r="149">
       <c r="A149" s="1"/>
@@ -2204,6 +2973,7 @@
       <c r="F149" s="1"/>
       <c r="G149" s="1"/>
       <c r="H149" s="1"/>
+      <c r="I149" s="1"/>
     </row>
     <row r="150">
       <c r="A150" s="1"/>
@@ -2214,6 +2984,7 @@
       <c r="F150" s="1"/>
       <c r="G150" s="1"/>
       <c r="H150" s="1"/>
+      <c r="I150" s="1"/>
     </row>
     <row r="151">
       <c r="A151" s="1"/>
@@ -2224,6 +2995,7 @@
       <c r="F151" s="1"/>
       <c r="G151" s="1"/>
       <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
     </row>
     <row r="152">
       <c r="A152" s="1"/>
@@ -2234,6 +3006,7 @@
       <c r="F152" s="1"/>
       <c r="G152" s="1"/>
       <c r="H152" s="1"/>
+      <c r="I152" s="1"/>
     </row>
     <row r="153">
       <c r="A153" s="1"/>
@@ -2244,6 +3017,7 @@
       <c r="F153" s="1"/>
       <c r="G153" s="1"/>
       <c r="H153" s="1"/>
+      <c r="I153" s="1"/>
     </row>
     <row r="154">
       <c r="A154" s="1"/>
@@ -2254,6 +3028,7 @@
       <c r="F154" s="1"/>
       <c r="G154" s="1"/>
       <c r="H154" s="1"/>
+      <c r="I154" s="1"/>
     </row>
     <row r="155">
       <c r="A155" s="1"/>
@@ -2264,6 +3039,7 @@
       <c r="F155" s="1"/>
       <c r="G155" s="1"/>
       <c r="H155" s="1"/>
+      <c r="I155" s="1"/>
     </row>
     <row r="156">
       <c r="A156" s="1"/>
@@ -2274,6 +3050,7 @@
       <c r="F156" s="1"/>
       <c r="G156" s="1"/>
       <c r="H156" s="1"/>
+      <c r="I156" s="1"/>
     </row>
     <row r="157">
       <c r="A157" s="1"/>
@@ -2284,6 +3061,7 @@
       <c r="F157" s="1"/>
       <c r="G157" s="1"/>
       <c r="H157" s="1"/>
+      <c r="I157" s="1"/>
     </row>
     <row r="158">
       <c r="A158" s="1"/>
@@ -2294,6 +3072,7 @@
       <c r="F158" s="1"/>
       <c r="G158" s="1"/>
       <c r="H158" s="1"/>
+      <c r="I158" s="1"/>
     </row>
     <row r="159">
       <c r="A159" s="1"/>
@@ -2304,6 +3083,7 @@
       <c r="F159" s="1"/>
       <c r="G159" s="1"/>
       <c r="H159" s="1"/>
+      <c r="I159" s="1"/>
     </row>
     <row r="160">
       <c r="A160" s="1"/>
@@ -2314,6 +3094,7 @@
       <c r="F160" s="1"/>
       <c r="G160" s="1"/>
       <c r="H160" s="1"/>
+      <c r="I160" s="1"/>
     </row>
     <row r="161">
       <c r="A161" s="1"/>
@@ -2324,6 +3105,7 @@
       <c r="F161" s="1"/>
       <c r="G161" s="1"/>
       <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
     </row>
     <row r="162">
       <c r="A162" s="1"/>
@@ -2334,6 +3116,7 @@
       <c r="F162" s="1"/>
       <c r="G162" s="1"/>
       <c r="H162" s="1"/>
+      <c r="I162" s="1"/>
     </row>
     <row r="163">
       <c r="A163" s="1"/>
@@ -2344,6 +3127,7 @@
       <c r="F163" s="1"/>
       <c r="G163" s="1"/>
       <c r="H163" s="1"/>
+      <c r="I163" s="1"/>
     </row>
     <row r="164">
       <c r="A164" s="1"/>
@@ -2354,6 +3138,7 @@
       <c r="F164" s="1"/>
       <c r="G164" s="1"/>
       <c r="H164" s="1"/>
+      <c r="I164" s="1"/>
     </row>
     <row r="165">
       <c r="A165" s="1"/>
@@ -2364,6 +3149,7 @@
       <c r="F165" s="1"/>
       <c r="G165" s="1"/>
       <c r="H165" s="1"/>
+      <c r="I165" s="1"/>
     </row>
     <row r="166">
       <c r="A166" s="1"/>
@@ -2374,6 +3160,7 @@
       <c r="F166" s="1"/>
       <c r="G166" s="1"/>
       <c r="H166" s="1"/>
+      <c r="I166" s="1"/>
     </row>
     <row r="167">
       <c r="A167" s="1"/>
@@ -2384,6 +3171,7 @@
       <c r="F167" s="1"/>
       <c r="G167" s="1"/>
       <c r="H167" s="1"/>
+      <c r="I167" s="1"/>
     </row>
     <row r="168">
       <c r="A168" s="1"/>
@@ -2394,6 +3182,7 @@
       <c r="F168" s="1"/>
       <c r="G168" s="1"/>
       <c r="H168" s="1"/>
+      <c r="I168" s="1"/>
     </row>
     <row r="169">
       <c r="A169" s="1"/>
@@ -2404,6 +3193,7 @@
       <c r="F169" s="1"/>
       <c r="G169" s="1"/>
       <c r="H169" s="1"/>
+      <c r="I169" s="1"/>
     </row>
     <row r="170">
       <c r="A170" s="1"/>
@@ -2414,6 +3204,7 @@
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
+      <c r="I170" s="1"/>
     </row>
     <row r="171">
       <c r="A171" s="1"/>
@@ -2424,6 +3215,7 @@
       <c r="F171" s="1"/>
       <c r="G171" s="1"/>
       <c r="H171" s="1"/>
+      <c r="I171" s="1"/>
     </row>
     <row r="172">
       <c r="A172" s="1"/>
@@ -2434,6 +3226,7 @@
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="1"/>
+      <c r="I172" s="1"/>
     </row>
     <row r="173">
       <c r="A173" s="1"/>
@@ -2444,6 +3237,7 @@
       <c r="F173" s="1"/>
       <c r="G173" s="1"/>
       <c r="H173" s="1"/>
+      <c r="I173" s="1"/>
     </row>
     <row r="174">
       <c r="A174" s="1"/>
@@ -2454,6 +3248,7 @@
       <c r="F174" s="1"/>
       <c r="G174" s="1"/>
       <c r="H174" s="1"/>
+      <c r="I174" s="1"/>
     </row>
     <row r="175">
       <c r="A175" s="1"/>
@@ -2464,6 +3259,7 @@
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="1"/>
+      <c r="I175" s="1"/>
     </row>
     <row r="176">
       <c r="A176" s="1"/>
@@ -2474,6 +3270,7 @@
       <c r="F176" s="1"/>
       <c r="G176" s="1"/>
       <c r="H176" s="1"/>
+      <c r="I176" s="1"/>
     </row>
     <row r="177">
       <c r="A177" s="1"/>
@@ -2484,6 +3281,7 @@
       <c r="F177" s="1"/>
       <c r="G177" s="1"/>
       <c r="H177" s="1"/>
+      <c r="I177" s="1"/>
     </row>
     <row r="178">
       <c r="A178" s="1"/>
@@ -2494,6 +3292,7 @@
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="1"/>
+      <c r="I178" s="1"/>
     </row>
     <row r="179">
       <c r="A179" s="1"/>
@@ -2504,6 +3303,7 @@
       <c r="F179" s="1"/>
       <c r="G179" s="1"/>
       <c r="H179" s="1"/>
+      <c r="I179" s="1"/>
     </row>
     <row r="180">
       <c r="A180" s="1"/>
@@ -2514,6 +3314,7 @@
       <c r="F180" s="1"/>
       <c r="G180" s="1"/>
       <c r="H180" s="1"/>
+      <c r="I180" s="1"/>
     </row>
     <row r="181">
       <c r="A181" s="1"/>
@@ -2524,6 +3325,7 @@
       <c r="F181" s="1"/>
       <c r="G181" s="1"/>
       <c r="H181" s="1"/>
+      <c r="I181" s="1"/>
     </row>
     <row r="182">
       <c r="A182" s="1"/>
@@ -2534,6 +3336,7 @@
       <c r="F182" s="1"/>
       <c r="G182" s="1"/>
       <c r="H182" s="1"/>
+      <c r="I182" s="1"/>
     </row>
     <row r="183">
       <c r="A183" s="1"/>
@@ -2544,6 +3347,7 @@
       <c r="F183" s="1"/>
       <c r="G183" s="1"/>
       <c r="H183" s="1"/>
+      <c r="I183" s="1"/>
     </row>
     <row r="184">
       <c r="A184" s="1"/>
@@ -2554,6 +3358,7 @@
       <c r="F184" s="1"/>
       <c r="G184" s="1"/>
       <c r="H184" s="1"/>
+      <c r="I184" s="1"/>
     </row>
     <row r="185">
       <c r="A185" s="1"/>
@@ -2564,6 +3369,7 @@
       <c r="F185" s="1"/>
       <c r="G185" s="1"/>
       <c r="H185" s="1"/>
+      <c r="I185" s="1"/>
     </row>
     <row r="186">
       <c r="A186" s="1"/>
@@ -2574,6 +3380,7 @@
       <c r="F186" s="1"/>
       <c r="G186" s="1"/>
       <c r="H186" s="1"/>
+      <c r="I186" s="1"/>
     </row>
     <row r="187">
       <c r="A187" s="1"/>
@@ -2584,6 +3391,7 @@
       <c r="F187" s="1"/>
       <c r="G187" s="1"/>
       <c r="H187" s="1"/>
+      <c r="I187" s="1"/>
     </row>
     <row r="188">
       <c r="A188" s="1"/>
@@ -2594,6 +3402,7 @@
       <c r="F188" s="1"/>
       <c r="G188" s="1"/>
       <c r="H188" s="1"/>
+      <c r="I188" s="1"/>
     </row>
     <row r="189">
       <c r="A189" s="1"/>
@@ -2604,6 +3413,7 @@
       <c r="F189" s="1"/>
       <c r="G189" s="1"/>
       <c r="H189" s="1"/>
+      <c r="I189" s="1"/>
     </row>
     <row r="190">
       <c r="A190" s="1"/>
@@ -2614,6 +3424,7 @@
       <c r="F190" s="1"/>
       <c r="G190" s="1"/>
       <c r="H190" s="1"/>
+      <c r="I190" s="1"/>
     </row>
     <row r="191">
       <c r="A191" s="1"/>
@@ -2624,6 +3435,7 @@
       <c r="F191" s="1"/>
       <c r="G191" s="1"/>
       <c r="H191" s="1"/>
+      <c r="I191" s="1"/>
     </row>
     <row r="192">
       <c r="A192" s="1"/>
@@ -2634,6 +3446,7 @@
       <c r="F192" s="1"/>
       <c r="G192" s="1"/>
       <c r="H192" s="1"/>
+      <c r="I192" s="1"/>
     </row>
     <row r="193">
       <c r="A193" s="1"/>
@@ -2644,6 +3457,7 @@
       <c r="F193" s="1"/>
       <c r="G193" s="1"/>
       <c r="H193" s="1"/>
+      <c r="I193" s="1"/>
     </row>
     <row r="194">
       <c r="A194" s="1"/>
@@ -2654,6 +3468,7 @@
       <c r="F194" s="1"/>
       <c r="G194" s="1"/>
       <c r="H194" s="1"/>
+      <c r="I194" s="1"/>
     </row>
     <row r="195">
       <c r="A195" s="1"/>
@@ -2664,6 +3479,7 @@
       <c r="F195" s="1"/>
       <c r="G195" s="1"/>
       <c r="H195" s="1"/>
+      <c r="I195" s="1"/>
     </row>
     <row r="196">
       <c r="A196" s="1"/>
@@ -2674,6 +3490,7 @@
       <c r="F196" s="1"/>
       <c r="G196" s="1"/>
       <c r="H196" s="1"/>
+      <c r="I196" s="1"/>
     </row>
     <row r="197">
       <c r="A197" s="1"/>
@@ -2684,6 +3501,7 @@
       <c r="F197" s="1"/>
       <c r="G197" s="1"/>
       <c r="H197" s="1"/>
+      <c r="I197" s="1"/>
     </row>
     <row r="198">
       <c r="A198" s="1"/>
@@ -2694,6 +3512,7 @@
       <c r="F198" s="1"/>
       <c r="G198" s="1"/>
       <c r="H198" s="1"/>
+      <c r="I198" s="1"/>
     </row>
     <row r="199">
       <c r="A199" s="1"/>
@@ -2704,6 +3523,7 @@
       <c r="F199" s="1"/>
       <c r="G199" s="1"/>
       <c r="H199" s="1"/>
+      <c r="I199" s="1"/>
     </row>
     <row r="200">
       <c r="A200" s="1"/>
@@ -2714,6 +3534,7 @@
       <c r="F200" s="1"/>
       <c r="G200" s="1"/>
       <c r="H200" s="1"/>
+      <c r="I200" s="1"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>

<commit_message>
adjust for build android project
</commit_message>
<xml_diff>
--- a/excelToJson/Value.xlsx
+++ b/excelToJson/Value.xlsx
@@ -462,22 +462,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>56</v>
+        <v>112</v>
       </c>
       <c r="F2" s="1">
         <v>8</v>
       </c>
       <c r="G2" s="1">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="H2" s="1">
         <v>12</v>
@@ -491,28 +491,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>267</v>
+        <v>720</v>
       </c>
       <c r="C3" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>112</v>
+        <v>224</v>
       </c>
       <c r="F3" s="1">
         <v>16</v>
       </c>
       <c r="G3" s="1">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="H3" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1">
-        <v>587</v>
+        <v>339</v>
       </c>
     </row>
     <row r="4">
@@ -520,28 +520,28 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>675</v>
+        <v>930</v>
       </c>
       <c r="C4" s="1">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>224</v>
+        <v>448</v>
       </c>
       <c r="F4" s="1">
         <v>32</v>
       </c>
       <c r="G4" s="1">
-        <v>88</v>
+        <v>240</v>
       </c>
       <c r="H4" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I4" s="1">
-        <v>781</v>
+        <v>410</v>
       </c>
     </row>
     <row r="5">
@@ -549,28 +549,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>778</v>
+        <v>2160</v>
       </c>
       <c r="C5" s="1">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D5" s="1">
         <v>4</v>
       </c>
       <c r="E5" s="1">
-        <v>448</v>
+        <v>896</v>
       </c>
       <c r="F5" s="1">
         <v>64</v>
       </c>
       <c r="G5" s="1">
-        <v>175</v>
+        <v>480</v>
       </c>
       <c r="H5" s="1">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="I5" s="1">
-        <v>1039</v>
+        <v>496</v>
       </c>
     </row>
     <row r="6">
@@ -578,28 +578,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>1800</v>
+        <v>3189</v>
       </c>
       <c r="C6" s="1">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="D6" s="1">
         <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>896</v>
+        <v>1792</v>
       </c>
       <c r="F6" s="1">
         <v>128</v>
       </c>
       <c r="G6" s="1">
-        <v>349</v>
+        <v>960</v>
       </c>
       <c r="H6" s="1">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="I6" s="1">
-        <v>1383</v>
+        <v>600</v>
       </c>
     </row>
     <row r="7">
@@ -607,28 +607,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>1338</v>
+        <v>2581</v>
       </c>
       <c r="C7" s="1">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="D7" s="1">
         <v>6</v>
       </c>
       <c r="E7" s="1">
-        <v>1792</v>
+        <v>3584</v>
       </c>
       <c r="F7" s="1">
         <v>256</v>
       </c>
       <c r="G7" s="1">
-        <v>697</v>
+        <v>1920</v>
       </c>
       <c r="H7" s="1">
-        <v>359</v>
+        <v>384</v>
       </c>
       <c r="I7" s="1">
-        <v>1841</v>
+        <v>725</v>
       </c>
     </row>
     <row r="8">
@@ -636,28 +636,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>1806</v>
+        <v>3188</v>
       </c>
       <c r="C8" s="1">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="D8" s="1">
         <v>7</v>
       </c>
       <c r="E8" s="1">
-        <v>3584</v>
+        <v>7168</v>
       </c>
       <c r="F8" s="1">
         <v>512</v>
       </c>
       <c r="G8" s="1">
-        <v>1393</v>
+        <v>3840</v>
       </c>
       <c r="H8" s="1">
-        <v>717</v>
+        <v>768</v>
       </c>
       <c r="I8" s="1">
-        <v>2450</v>
+        <v>878</v>
       </c>
     </row>
     <row r="9">
@@ -665,28 +665,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>2507</v>
+        <v>5885</v>
       </c>
       <c r="C9" s="1">
-        <v>160</v>
+        <v>102</v>
       </c>
       <c r="D9" s="1">
         <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>7168</v>
+        <v>14336</v>
       </c>
       <c r="F9" s="1">
         <v>1024</v>
       </c>
       <c r="G9" s="1">
-        <v>2786</v>
-      </c>
-      <c r="H9" s="1">
-        <v>1434</v>
+        <v>7680</v>
+      </c>
+      <c r="H9" s="1" t="str">
+        <v>#REF!</v>
       </c>
       <c r="I9" s="1">
-        <v>3261</v>
+        <v>1062</v>
       </c>
     </row>
     <row r="10">
@@ -694,28 +694,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>2995</v>
+        <v>6117</v>
       </c>
       <c r="C10" s="1">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="D10" s="1">
         <v>9</v>
       </c>
       <c r="E10" s="1">
-        <v>14336</v>
+        <v>28672</v>
       </c>
       <c r="F10" s="1">
         <v>2048</v>
       </c>
       <c r="G10" s="1">
-        <v>5571</v>
+        <v>15360</v>
       </c>
       <c r="H10" s="1">
-        <v>2868</v>
+        <v>3072</v>
       </c>
       <c r="I10" s="1">
-        <v>4340</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="11">
@@ -723,10 +723,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>4616</v>
+        <v>8562</v>
       </c>
       <c r="C11" s="1">
-        <v>164</v>
+        <v>132</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -734,7 +734,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1">
-        <v>5776</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="12">
@@ -742,10 +742,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>4740</v>
+        <v>6687</v>
       </c>
       <c r="C12" s="1">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -753,7 +753,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1">
-        <v>7688</v>
+        <v>1881</v>
       </c>
     </row>
     <row r="13">
@@ -761,10 +761,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>4853</v>
+        <v>9230</v>
       </c>
       <c r="C13" s="1">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -772,7 +772,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1">
-        <v>10233</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="14">
@@ -780,10 +780,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>5931</v>
+        <v>10834</v>
       </c>
       <c r="C14" s="1">
-        <v>313</v>
+        <v>180</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -791,7 +791,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1">
-        <v>13619</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="15">
@@ -799,10 +799,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>6047</v>
+        <v>11890</v>
       </c>
       <c r="C15" s="1">
-        <v>315</v>
+        <v>186</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -810,7 +810,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1">
-        <v>18127</v>
+        <v>3332</v>
       </c>
     </row>
     <row r="16">
@@ -818,10 +818,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>10377</v>
+        <v>14651</v>
       </c>
       <c r="C16" s="1">
-        <v>317</v>
+        <v>204</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -829,7 +829,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1">
-        <v>24127</v>
+        <v>4031</v>
       </c>
     </row>
     <row r="17">
@@ -837,10 +837,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>9503</v>
+        <v>12002</v>
       </c>
       <c r="C17" s="1">
-        <v>319</v>
+        <v>222</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -848,7 +848,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1">
-        <v>32113</v>
+        <v>4878</v>
       </c>
     </row>
     <row r="18">
@@ -856,10 +856,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>10729</v>
+        <v>15327</v>
       </c>
       <c r="C18" s="1">
-        <v>321</v>
+        <v>240</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -867,7 +867,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1">
-        <v>42743</v>
+        <v>5902</v>
       </c>
     </row>
     <row r="19">
@@ -875,10 +875,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>10888</v>
+        <v>17711</v>
       </c>
       <c r="C19" s="1">
-        <v>323</v>
+        <v>258</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -886,7 +886,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1">
-        <v>56890</v>
+        <v>7141</v>
       </c>
     </row>
     <row r="20">
@@ -894,10 +894,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>11145</v>
+        <v>18028</v>
       </c>
       <c r="C20" s="1">
-        <v>325</v>
+        <v>276</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -905,7 +905,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1">
-        <v>75721</v>
+        <v>8641</v>
       </c>
     </row>
     <row r="21">
@@ -913,10 +913,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>11504</v>
+        <v>26950</v>
       </c>
       <c r="C21" s="1">
-        <v>327</v>
+        <v>294</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -924,7 +924,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1">
-        <v>100784</v>
+        <v>10455</v>
       </c>
     </row>
     <row r="22">
@@ -932,10 +932,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>11609</v>
+        <v>16417</v>
       </c>
       <c r="C22" s="1">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -943,7 +943,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1">
-        <v>134143</v>
+        <v>12651</v>
       </c>
     </row>
     <row r="23">
@@ -951,10 +951,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>14032</v>
+        <v>22200</v>
       </c>
       <c r="C23" s="1">
-        <v>617</v>
+        <v>330</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -962,7 +962,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1">
-        <v>178544</v>
+        <v>15308</v>
       </c>
     </row>
     <row r="24">
@@ -970,10 +970,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>21222</v>
+        <v>28118</v>
       </c>
       <c r="C24" s="1">
-        <v>619</v>
+        <v>347</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
@@ -981,7 +981,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1">
-        <v>237643</v>
+        <v>18522</v>
       </c>
     </row>
     <row r="25">
@@ -989,10 +989,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>23766</v>
+        <v>28467</v>
       </c>
       <c r="C25" s="1">
-        <v>621</v>
+        <v>366</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -1000,7 +1000,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1">
-        <v>316302</v>
+        <v>22411</v>
       </c>
     </row>
     <row r="26">
@@ -1008,10 +1008,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>28943</v>
+        <v>34688</v>
       </c>
       <c r="C26" s="1">
-        <v>623</v>
+        <v>390</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -1019,7 +1019,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1">
-        <v>420998</v>
+        <v>47017</v>
       </c>
     </row>
     <row r="27">
@@ -1027,10 +1027,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>24311</v>
+        <v>28148</v>
       </c>
       <c r="C27" s="1">
-        <v>625</v>
+        <v>414</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -1038,7 +1038,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1">
-        <v>560348</v>
+        <v>62579</v>
       </c>
     </row>
     <row r="28">
@@ -1046,10 +1046,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>26945</v>
+        <v>35653</v>
       </c>
       <c r="C28" s="1">
-        <v>627</v>
+        <v>438</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -1057,7 +1057,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1">
-        <v>745823</v>
+        <v>83293</v>
       </c>
     </row>
     <row r="29">
@@ -1065,10 +1065,10 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>29609</v>
+        <v>36096</v>
       </c>
       <c r="C29" s="1">
-        <v>629</v>
+        <v>462</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -1076,7 +1076,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1">
-        <v>992690</v>
+        <v>110862</v>
       </c>
     </row>
     <row r="30">
@@ -1084,10 +1084,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="1">
-        <v>32300</v>
+        <v>36517</v>
       </c>
       <c r="C30" s="1">
-        <v>631</v>
+        <v>486</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -1095,7 +1095,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1">
-        <v>1321271</v>
+        <v>147558</v>
       </c>
     </row>
     <row r="31">
@@ -1103,10 +1103,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="1">
-        <v>40592</v>
+        <v>49224</v>
       </c>
       <c r="C31" s="1">
-        <v>633</v>
+        <v>510</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -1114,7 +1114,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1">
-        <v>1758611</v>
+        <v>196399</v>
       </c>
     </row>
     <row r="32">
@@ -1122,10 +1122,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="1">
-        <v>35677</v>
+        <v>37393</v>
       </c>
       <c r="C32" s="1">
-        <v>635</v>
+        <v>540</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -1133,7 +1133,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1">
-        <v>2340711</v>
+        <v>261407</v>
       </c>
     </row>
     <row r="33">
@@ -1141,10 +1141,10 @@
         <v>32</v>
       </c>
       <c r="B33" s="1">
-        <v>35833</v>
+        <v>37842</v>
       </c>
       <c r="C33" s="1">
-        <v>637</v>
+        <v>570</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1152,7 +1152,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1">
-        <v>3115486</v>
+        <v>347932</v>
       </c>
     </row>
     <row r="34">
@@ -1160,10 +1160,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>35985</v>
+        <v>38268</v>
       </c>
       <c r="C34" s="1">
-        <v>639</v>
+        <v>600</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1171,7 +1171,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1">
-        <v>4146712</v>
+        <v>463098</v>
       </c>
     </row>
     <row r="35">
@@ -1179,10 +1179,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>36135</v>
+        <v>38674</v>
       </c>
       <c r="C35" s="1">
-        <v>641</v>
+        <v>629</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -1190,7 +1190,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1">
-        <v>5519274</v>
+        <v>616383</v>
       </c>
     </row>
     <row r="36">
@@ -1198,10 +1198,10 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>36377</v>
+        <v>52080</v>
       </c>
       <c r="C36" s="1">
-        <v>643</v>
+        <v>660</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -1209,7 +1209,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="1">
-        <v>7346153</v>
+        <v>820405</v>
       </c>
     </row>
     <row r="37">
@@ -1217,10 +1217,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>26101</v>
+        <v>39284</v>
       </c>
       <c r="C37" s="1">
-        <v>645</v>
+        <v>678</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -1228,7 +1228,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="1">
-        <v>9777729</v>
+        <v>1091959</v>
       </c>
     </row>
     <row r="38">
@@ -1236,10 +1236,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>26216</v>
+        <v>39573</v>
       </c>
       <c r="C38" s="1">
-        <v>647</v>
+        <v>702</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -1247,7 +1247,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="1">
-        <v>13014158</v>
+        <v>1453398</v>
       </c>
     </row>
     <row r="39">
@@ -1255,10 +1255,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>26329</v>
+        <v>39852</v>
       </c>
       <c r="C39" s="1">
-        <v>649</v>
+        <v>726</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -1266,7 +1266,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
       <c r="I39" s="1">
-        <v>17321844</v>
+        <v>1934472</v>
       </c>
     </row>
     <row r="40">
@@ -1274,10 +1274,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>26439</v>
+        <v>40056</v>
       </c>
       <c r="C40" s="1">
-        <v>651</v>
+        <v>744</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -1285,7 +1285,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
       <c r="I40" s="1">
-        <v>23055374</v>
+        <v>2574782</v>
       </c>
     </row>
     <row r="41">
@@ -1293,10 +1293,10 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>42834</v>
+        <v>80897</v>
       </c>
       <c r="C41" s="1">
-        <v>653</v>
+        <v>780</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -1304,7 +1304,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="1">
-        <v>30686702</v>
+        <v>3427035</v>
       </c>
     </row>
     <row r="42">
@@ -1312,10 +1312,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>26858</v>
+        <v>81647</v>
       </c>
       <c r="C42" s="1">
-        <v>655</v>
+        <v>816</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -1323,7 +1323,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
       <c r="I42" s="1">
-        <v>40844001</v>
+        <v>4561383</v>
       </c>
     </row>
     <row r="43">
@@ -1331,10 +1331,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>28021</v>
+        <v>82365</v>
       </c>
       <c r="C43" s="1">
-        <v>1231</v>
+        <v>852</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -1342,7 +1342,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="1">
-        <v>54363365</v>
+        <v>6071201</v>
       </c>
     </row>
     <row r="44">
@@ -1350,10 +1350,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>32433</v>
+        <v>83052</v>
       </c>
       <c r="C44" s="1">
-        <v>1233</v>
+        <v>887</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -1361,7 +1361,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
       <c r="I44" s="1">
-        <v>72357638</v>
+        <v>8080768</v>
       </c>
     </row>
     <row r="45">
@@ -1369,10 +1369,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>37954</v>
+        <v>83713</v>
       </c>
       <c r="C45" s="1">
-        <v>1235</v>
+        <v>924</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -1380,7 +1380,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1">
-        <v>96308016</v>
+        <v>10755502</v>
       </c>
     </row>
     <row r="46">
@@ -1388,10 +1388,10 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>54384</v>
+        <v>112464</v>
       </c>
       <c r="C46" s="1">
-        <v>1237</v>
+        <v>959</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -1399,7 +1399,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1">
-        <v>128185969</v>
+        <v>14315573</v>
       </c>
     </row>
     <row r="47">
@@ -1407,10 +1407,10 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>54597</v>
+        <v>84960</v>
       </c>
       <c r="C47" s="1">
-        <v>1239</v>
+        <v>996</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -1418,7 +1418,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1">
-        <v>170615525</v>
+        <v>19054028</v>
       </c>
     </row>
     <row r="48">
@@ -1426,10 +1426,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>54806</v>
+        <v>85550</v>
       </c>
       <c r="C48" s="1">
-        <v>1241</v>
+        <v>1032</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -1437,7 +1437,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
       <c r="I48" s="1">
-        <v>227089264</v>
+        <v>25360911</v>
       </c>
     </row>
     <row r="49">
@@ -1445,10 +1445,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>55011</v>
+        <v>86120</v>
       </c>
       <c r="C49" s="1">
-        <v>1243</v>
+        <v>1068</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -1456,7 +1456,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1">
-        <v>302255810</v>
+        <v>33755372</v>
       </c>
     </row>
     <row r="50">
@@ -1464,10 +1464,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>55212</v>
+        <v>86671</v>
       </c>
       <c r="C50" s="1">
-        <v>1245</v>
+        <v>1104</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -1475,7 +1475,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1">
-        <v>402302483</v>
+        <v>44928401</v>
       </c>
     </row>
     <row r="51">
@@ -1483,10 +1483,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>66491</v>
+        <v>116272</v>
       </c>
       <c r="C51" s="1">
-        <v>1247</v>
+        <v>1140</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1494,7 +1494,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1">
-        <v>535464604</v>
+        <v>92230650</v>
       </c>
     </row>
     <row r="52">
@@ -1502,10 +1502,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1">
-        <v>55554</v>
+        <v>87806</v>
       </c>
       <c r="C52" s="1">
-        <v>1249</v>
+        <v>1182</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -1513,7 +1513,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1">
-        <v>712703388</v>
+        <v>135034895</v>
       </c>
     </row>
     <row r="53">
@@ -1521,10 +1521,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1">
-        <v>55697</v>
+        <v>88386</v>
       </c>
       <c r="C53" s="1">
-        <v>1251</v>
+        <v>1223</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -1532,7 +1532,7 @@
       <c r="G53" s="1"/>
       <c r="H53" s="1"/>
       <c r="I53" s="1">
-        <v>948608209</v>
+        <v>197704589</v>
       </c>
     </row>
     <row r="54">
@@ -1540,10 +1540,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="1">
-        <v>55839</v>
+        <v>88947</v>
       </c>
       <c r="C54" s="1">
-        <v>1253</v>
+        <v>1266</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -1551,7 +1551,7 @@
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
       <c r="I54" s="1">
-        <v>1262597526</v>
+        <v>289459289</v>
       </c>
     </row>
     <row r="55">
@@ -1559,10 +1559,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1">
-        <v>55978</v>
+        <v>89489</v>
       </c>
       <c r="C55" s="1">
-        <v>1255</v>
+        <v>1307</v>
       </c>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -1570,7 +1570,7 @@
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
       <c r="I55" s="1">
-        <v>1680517307</v>
+        <v>423797345</v>
       </c>
     </row>
     <row r="56">
@@ -1578,10 +1578,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>67339</v>
+        <v>120019</v>
       </c>
       <c r="C56" s="1">
-        <v>1257</v>
+        <v>1350</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -1589,7 +1589,7 @@
       <c r="G56" s="1"/>
       <c r="H56" s="1"/>
       <c r="I56" s="1">
-        <v>2236768536</v>
+        <v>620481693</v>
       </c>
     </row>
     <row r="57">
@@ -1597,10 +1597,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1">
-        <v>56274</v>
+        <v>90523</v>
       </c>
       <c r="C57" s="1">
-        <v>1259</v>
+        <v>1391</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -1608,7 +1608,7 @@
       <c r="G57" s="1"/>
       <c r="H57" s="1"/>
       <c r="I57" s="1">
-        <v>2977138921</v>
+        <v>908447246</v>
       </c>
     </row>
     <row r="58">
@@ -1616,10 +1616,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="1">
-        <v>56430</v>
+        <v>91017</v>
       </c>
       <c r="C58" s="1">
-        <v>1261</v>
+        <v>1434</v>
       </c>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -1627,7 +1627,7 @@
       <c r="G58" s="1"/>
       <c r="H58" s="1"/>
       <c r="I58" s="1">
-        <v>3962571904</v>
+        <v>1330057613</v>
       </c>
     </row>
     <row r="59">
@@ -1635,10 +1635,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="1">
-        <v>56584</v>
+        <v>91497</v>
       </c>
       <c r="C59" s="1">
-        <v>1263</v>
+        <v>1476</v>
       </c>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -1646,7 +1646,7 @@
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="1">
-        <v>5274183204</v>
+        <v>1947337351</v>
       </c>
     </row>
     <row r="60">
@@ -1654,10 +1654,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>56735</v>
+        <v>91964</v>
       </c>
       <c r="C60" s="1">
-        <v>1265</v>
+        <v>1518</v>
       </c>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -1665,7 +1665,7 @@
       <c r="G60" s="1"/>
       <c r="H60" s="1"/>
       <c r="I60" s="1">
-        <v>7019937844</v>
+        <v>2851096615</v>
       </c>
     </row>
     <row r="61">
@@ -1673,10 +1673,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1">
-        <v>74356</v>
+        <v>184835</v>
       </c>
       <c r="C61" s="1">
-        <v>1267</v>
+        <v>1560</v>
       </c>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -1684,7 +1684,7 @@
       <c r="G61" s="1"/>
       <c r="H61" s="1"/>
       <c r="I61" s="1">
-        <v>9343537270</v>
+        <v>6040273084</v>
       </c>
     </row>
     <row r="62">
@@ -1692,10 +1692,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1">
-        <v>57339</v>
+        <v>185842</v>
       </c>
       <c r="C62" s="1">
-        <v>1269</v>
+        <v>1607</v>
       </c>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -1703,7 +1703,7 @@
       <c r="G62" s="1"/>
       <c r="H62" s="1"/>
       <c r="I62" s="1">
-        <v>12436248106</v>
+        <v>9727920204</v>
       </c>
     </row>
     <row r="63">
@@ -1711,10 +1711,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="1">
-        <v>57480</v>
+        <v>186820</v>
       </c>
       <c r="C63" s="1">
-        <v>1271</v>
+        <v>1655</v>
       </c>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -1722,7 +1722,7 @@
       <c r="G63" s="1"/>
       <c r="H63" s="1"/>
       <c r="I63" s="1">
-        <v>16552646230</v>
+        <v>15666912768</v>
       </c>
     </row>
     <row r="64">
@@ -1730,10 +1730,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>57619</v>
+        <v>187770</v>
       </c>
       <c r="C64" s="1">
-        <v>1273</v>
+        <v>1704</v>
       </c>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -1741,7 +1741,7 @@
       <c r="G64" s="1"/>
       <c r="H64" s="1"/>
       <c r="I64" s="1">
-        <v>22031572131</v>
+        <v>25231719681</v>
       </c>
     </row>
     <row r="65">
@@ -1749,10 +1749,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="1">
-        <v>57756</v>
+        <v>188693</v>
       </c>
       <c r="C65" s="1">
-        <v>1275</v>
+        <v>1752</v>
       </c>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -1760,7 +1760,7 @@
       <c r="G65" s="1"/>
       <c r="H65" s="1"/>
       <c r="I65" s="1">
-        <v>29324022507</v>
+        <v>40635936863</v>
       </c>
     </row>
     <row r="66">
@@ -1768,10 +1768,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="1">
-        <v>69469</v>
+        <v>252789</v>
       </c>
       <c r="C66" s="1">
-        <v>1277</v>
+        <v>1800</v>
       </c>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -1779,7 +1779,7 @@
       <c r="G66" s="1"/>
       <c r="H66" s="1"/>
       <c r="I66" s="1">
-        <v>39030273956</v>
+        <v>65444582678</v>
       </c>
     </row>
     <row r="67">
@@ -1787,10 +1787,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1">
-        <v>58043</v>
+        <v>190466</v>
       </c>
       <c r="C67" s="1">
-        <v>1279</v>
+        <v>1848</v>
       </c>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -1798,7 +1798,7 @@
       <c r="G67" s="1"/>
       <c r="H67" s="1"/>
       <c r="I67" s="1">
-        <v>51949294636</v>
+        <v>105399154848</v>
       </c>
     </row>
     <row r="68">
@@ -1806,10 +1806,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
-        <v>58194</v>
+        <v>191319</v>
       </c>
       <c r="C68" s="1">
-        <v>1281</v>
+        <v>1896</v>
       </c>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -1817,7 +1817,7 @@
       <c r="G68" s="1"/>
       <c r="H68" s="1"/>
       <c r="I68" s="1">
-        <v>69144511160</v>
+        <v>169746392873</v>
       </c>
     </row>
     <row r="69">
@@ -1825,10 +1825,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
-        <v>58342</v>
+        <v>192150</v>
       </c>
       <c r="C69" s="1">
-        <v>1283</v>
+        <v>1943</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -1836,7 +1836,7 @@
       <c r="G69" s="1"/>
       <c r="H69" s="1"/>
       <c r="I69" s="1">
-        <v>92031344353</v>
+        <v>273378263186</v>
       </c>
     </row>
     <row r="70">
@@ -1844,10 +1844,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
-        <v>58488</v>
+        <v>192960</v>
       </c>
       <c r="C70" s="1">
-        <v>1285</v>
+        <v>1991</v>
       </c>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -1855,7 +1855,7 @@
       <c r="G70" s="1"/>
       <c r="H70" s="1"/>
       <c r="I70" s="1">
-        <v>122493719334</v>
+        <v>440278426644</v>
       </c>
     </row>
     <row r="71">
@@ -1863,10 +1863,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
-        <v>82258</v>
+        <v>322920</v>
       </c>
       <c r="C71" s="1">
-        <v>1287</v>
+        <v>2040</v>
       </c>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -1874,7 +1874,7 @@
       <c r="G71" s="1"/>
       <c r="H71" s="1"/>
       <c r="I71" s="1">
-        <v>163039140434</v>
+        <v>985736872538</v>
       </c>
     </row>
     <row r="72">
@@ -1882,10 +1882,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
-        <v>58896</v>
+        <v>194620</v>
       </c>
       <c r="C72" s="1">
-        <v>1289</v>
+        <v>2094</v>
       </c>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -1893,7 +1893,7 @@
       <c r="G72" s="1"/>
       <c r="H72" s="1"/>
       <c r="I72" s="1">
-        <v>217005095917</v>
+        <v>1746292999650</v>
       </c>
     </row>
     <row r="73">
@@ -1901,10 +1901,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
-        <v>59035</v>
+        <v>195467</v>
       </c>
       <c r="C73" s="1">
-        <v>1291</v>
+        <v>2148</v>
       </c>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -1912,7 +1912,7 @@
       <c r="G73" s="1"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1">
-        <v>288833782666</v>
+        <v>3093664572752</v>
       </c>
     </row>
     <row r="74">
@@ -1920,10 +1920,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
-        <v>59171</v>
+        <v>196292</v>
       </c>
       <c r="C74" s="1">
-        <v>1293</v>
+        <v>2202</v>
       </c>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -1931,7 +1931,7 @@
       <c r="G74" s="1"/>
       <c r="H74" s="1"/>
       <c r="I74" s="1">
-        <v>384437764728</v>
+        <v>5480615504168</v>
       </c>
     </row>
     <row r="75">
@@ -1939,10 +1939,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="1">
-        <v>59306</v>
+        <v>197097</v>
       </c>
       <c r="C75" s="1">
-        <v>1295</v>
+        <v>2256</v>
       </c>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -1950,7 +1950,7 @@
       <c r="G75" s="1"/>
       <c r="H75" s="1"/>
       <c r="I75" s="1">
-        <v>511686664853</v>
+        <v>9709244683179</v>
       </c>
     </row>
     <row r="76">
@@ -1958,10 +1958,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="1">
-        <v>77271</v>
+        <v>263845</v>
       </c>
       <c r="C76" s="1">
-        <v>1297</v>
+        <v>2310</v>
       </c>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -1969,7 +1969,7 @@
       <c r="G76" s="1"/>
       <c r="H76" s="1"/>
       <c r="I76" s="1">
-        <v>681054950919</v>
+        <v>17200519220177</v>
       </c>
     </row>
     <row r="77">
@@ -1977,10 +1977,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
-        <v>59603</v>
+        <v>198652</v>
       </c>
       <c r="C77" s="1">
-        <v>1299</v>
+        <v>2364</v>
       </c>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -1988,7 +1988,7 @@
       <c r="G77" s="1"/>
       <c r="H77" s="1"/>
       <c r="I77" s="1">
-        <v>906484139672</v>
+        <v>30471769030216</v>
       </c>
     </row>
     <row r="78">
@@ -1996,10 +1996,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <v>59764</v>
+        <v>199402</v>
       </c>
       <c r="C78" s="1">
-        <v>1301</v>
+        <v>2418</v>
       </c>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -2007,7 +2007,7 @@
       <c r="G78" s="1"/>
       <c r="H78" s="1"/>
       <c r="I78" s="1">
-        <v>1206530389904</v>
+        <v>53982597614939</v>
       </c>
     </row>
     <row r="79">
@@ -2015,10 +2015,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <v>59923</v>
+        <v>200136</v>
       </c>
       <c r="C79" s="1">
-        <v>1303</v>
+        <v>2472</v>
       </c>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
@@ -2026,7 +2026,7 @@
       <c r="G79" s="1"/>
       <c r="H79" s="1"/>
       <c r="I79" s="1">
-        <v>1605891948962</v>
+        <v>95633464613318</v>
       </c>
     </row>
     <row r="80">
@@ -2034,10 +2034,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="1">
-        <v>60080</v>
+        <v>200855</v>
       </c>
       <c r="C80" s="1">
-        <v>1305</v>
+        <v>2525</v>
       </c>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
@@ -2045,7 +2045,7 @@
       <c r="G80" s="1"/>
       <c r="H80" s="1"/>
       <c r="I80" s="1">
-        <v>2137442184068</v>
+        <v>169420516203834</v>
       </c>
     </row>
     <row r="81">
@@ -2053,10 +2053,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="1">
-        <v>84413</v>
+        <v>335930</v>
       </c>
       <c r="C81" s="1">
-        <v>1307</v>
+        <v>2579</v>
       </c>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
@@ -2064,7 +2064,7 @@
       <c r="G81" s="1"/>
       <c r="H81" s="1"/>
       <c r="I81" s="1">
-        <v>2844935546994</v>
+        <v>405958143714741</v>
       </c>
     </row>
     <row r="82">
@@ -2072,10 +2072,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
-        <v>60401</v>
+        <v>202322</v>
       </c>
       <c r="C82" s="1">
-        <v>1309</v>
+        <v>2640</v>
       </c>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
@@ -2083,7 +2083,7 @@
       <c r="G82" s="1"/>
       <c r="H82" s="1"/>
       <c r="I82" s="1">
-        <v>3786609213049</v>
+        <v>791097576541173</v>
       </c>
     </row>
     <row r="83">
@@ -2091,10 +2091,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
-        <v>60506</v>
+        <v>203069</v>
       </c>
       <c r="C83" s="1">
-        <v>1311</v>
+        <v>2700</v>
       </c>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
@@ -2102,7 +2102,7 @@
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
       <c r="I83" s="1">
-        <v>5039976862569</v>
+        <v>1541625375174343</v>
       </c>
     </row>
     <row r="84">
@@ -2110,10 +2110,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
-        <v>60609</v>
+        <v>203800</v>
       </c>
       <c r="C84" s="1">
-        <v>1313</v>
+        <v>2760</v>
       </c>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
@@ -2121,7 +2121,7 @@
       <c r="G84" s="1"/>
       <c r="H84" s="1"/>
       <c r="I84" s="1">
-        <v>6708209204079</v>
+        <v>3004191730396158</v>
       </c>
     </row>
     <row r="85">
@@ -2129,10 +2129,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="1">
-        <v>60712</v>
+        <v>204514</v>
       </c>
       <c r="C85" s="1">
-        <v>1315</v>
+        <v>2819</v>
       </c>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
@@ -2140,7 +2140,7 @@
       <c r="G85" s="1"/>
       <c r="H85" s="1"/>
       <c r="I85" s="1">
-        <v>8928626450629</v>
+        <v>5854319796701586</v>
       </c>
     </row>
     <row r="86">
@@ -2148,10 +2148,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
-        <v>97555</v>
+        <v>273619</v>
       </c>
       <c r="C86" s="1">
-        <v>2464</v>
+        <v>2880</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -2159,7 +2159,7 @@
       <c r="G86" s="1"/>
       <c r="H86" s="1"/>
       <c r="I86" s="1">
-        <v>11884001805786</v>
+        <v>11408413096700912</v>
       </c>
     </row>
     <row r="87">
@@ -2167,10 +2167,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
-        <v>83076</v>
+        <v>205900</v>
       </c>
       <c r="C87" s="1">
-        <v>2466</v>
+        <v>2940</v>
       </c>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
@@ -2178,7 +2178,7 @@
       <c r="G87" s="1"/>
       <c r="H87" s="1"/>
       <c r="I87" s="1">
-        <v>15817606403502</v>
+        <v>22231769685405030</v>
       </c>
     </row>
     <row r="88">
@@ -2186,10 +2186,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
-        <v>97916</v>
+        <v>206571</v>
       </c>
       <c r="C88" s="1">
-        <v>2468</v>
+        <v>3000</v>
       </c>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
@@ -2197,7 +2197,7 @@
       <c r="G88" s="1"/>
       <c r="H88" s="1"/>
       <c r="I88" s="1">
-        <v>21053234123061</v>
+        <v>43323429749210424</v>
       </c>
     </row>
     <row r="89">
@@ -2205,10 +2205,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
-        <v>122617</v>
+        <v>207229</v>
       </c>
       <c r="C89" s="1">
-        <v>2470</v>
+        <v>3060</v>
       </c>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
@@ -2216,7 +2216,7 @@
       <c r="G89" s="1"/>
       <c r="H89" s="1"/>
       <c r="I89" s="1">
-        <v>28021854617793</v>
+        <v>84425108382935120</v>
       </c>
     </row>
     <row r="90">
@@ -2224,10 +2224,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
-        <v>122837</v>
+        <v>207295</v>
       </c>
       <c r="C90" s="1">
-        <v>2472</v>
+        <v>3066</v>
       </c>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
@@ -2235,7 +2235,7 @@
       <c r="G90" s="1"/>
       <c r="H90" s="1"/>
       <c r="I90" s="1">
-        <v>37297088496283</v>
+        <v>164520652375179100</v>
       </c>
     </row>
     <row r="91">
@@ -2243,10 +2243,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
-        <v>147923</v>
+        <v>415878</v>
       </c>
       <c r="C91" s="1">
-        <v>2474</v>
+        <v>3126</v>
       </c>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
@@ -2254,7 +2254,7 @@
       <c r="G91" s="1"/>
       <c r="H91" s="1"/>
       <c r="I91" s="1">
-        <v>49642424788552</v>
+        <v>425103883883278400</v>
       </c>
     </row>
     <row r="92">
@@ -2262,10 +2262,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
-        <v>123482</v>
+        <v>417267</v>
       </c>
       <c r="C92" s="1">
-        <v>2476</v>
+        <v>3192</v>
       </c>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
@@ -2273,7 +2273,7 @@
       <c r="G92" s="1"/>
       <c r="H92" s="1"/>
       <c r="I92" s="1">
-        <v>66074067393563</v>
+        <v>911247928579735600</v>
       </c>
     </row>
     <row r="93">
@@ -2281,10 +2281,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
-        <v>136061</v>
+        <v>418627</v>
       </c>
       <c r="C93" s="1">
-        <v>2478</v>
+        <v>3258</v>
       </c>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
@@ -2292,7 +2292,7 @@
       <c r="G93" s="1"/>
       <c r="H93" s="1"/>
       <c r="I93" s="1">
-        <v>87944583700832</v>
+        <v>1953340862839201500</v>
       </c>
     </row>
     <row r="94">
@@ -2300,10 +2300,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="1">
-        <v>142486</v>
+        <v>419961</v>
       </c>
       <c r="C94" s="1">
-        <v>2480</v>
+        <v>3324</v>
       </c>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
@@ -2311,7 +2311,7 @@
       <c r="G94" s="1"/>
       <c r="H94" s="1"/>
       <c r="I94" s="1">
-        <v>117054240905808</v>
+        <v>4187159615697859000</v>
       </c>
     </row>
     <row r="95">
@@ -2319,10 +2319,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="1">
-        <v>148928</v>
+        <v>421268</v>
       </c>
       <c r="C95" s="1">
-        <v>2482</v>
+        <v>3390</v>
       </c>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
@@ -2330,7 +2330,7 @@
       <c r="G95" s="1"/>
       <c r="H95" s="1"/>
       <c r="I95" s="1">
-        <v>155799194645630</v>
+        <v>8975548497893838000</v>
       </c>
     </row>
     <row r="96">
@@ -2338,10 +2338,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="1">
-        <v>166916</v>
+        <v>563400</v>
       </c>
       <c r="C96" s="1">
-        <v>2484</v>
+        <v>3456</v>
       </c>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
@@ -2349,7 +2349,7 @@
       <c r="G96" s="1"/>
       <c r="H96" s="1"/>
       <c r="I96" s="1">
-        <v>207368728073333</v>
+        <v>19239885323697553000</v>
       </c>
     </row>
     <row r="97">
@@ -2357,10 +2357,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="1">
-        <v>124764</v>
+        <v>423807</v>
       </c>
       <c r="C97" s="1">
-        <v>2486</v>
+        <v>3522</v>
       </c>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
@@ -2368,7 +2368,7 @@
       <c r="G97" s="1"/>
       <c r="H97" s="1"/>
       <c r="I97" s="1">
-        <v>276007777065606</v>
+        <v>41242402885561330000</v>
       </c>
     </row>
     <row r="98">
@@ -2376,10 +2376,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="1">
-        <v>124962</v>
+        <v>425041</v>
       </c>
       <c r="C98" s="1">
-        <v>2488</v>
+        <v>3587</v>
       </c>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
@@ -2387,7 +2387,7 @@
       <c r="G98" s="1"/>
       <c r="H98" s="1"/>
       <c r="I98" s="1">
-        <v>367366351274322</v>
+        <v>88406753323001040000</v>
       </c>
     </row>
     <row r="99">
@@ -2395,10 +2395,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="1">
-        <v>125158</v>
+        <v>426253</v>
       </c>
       <c r="C99" s="1">
-        <v>2490</v>
+        <v>3654</v>
       </c>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
@@ -2406,7 +2406,7 @@
       <c r="G99" s="1"/>
       <c r="H99" s="1"/>
       <c r="I99" s="1">
-        <v>488964613546122</v>
+        <v>189507727151615480000</v>
       </c>
     </row>
     <row r="100">
@@ -2414,10 +2414,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="1">
-        <v>125352</v>
+        <v>427443</v>
       </c>
       <c r="C100" s="1">
-        <v>2492</v>
+        <v>3720</v>
       </c>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
@@ -2425,7 +2425,7 @@
       <c r="G100" s="1"/>
       <c r="H100" s="1"/>
       <c r="I100" s="1">
-        <v>650811900629889</v>
+        <v>406226643330736260000</v>
       </c>
     </row>
     <row r="101">
@@ -2433,10 +2433,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>200872</v>
+        <v>857225</v>
       </c>
       <c r="C101" s="1">
-        <v>2494</v>
+        <v>3786</v>
       </c>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
@@ -2444,7 +2444,7 @@
       <c r="G101" s="1"/>
       <c r="H101" s="1"/>
       <c r="I101" s="1">
-        <v>866230639738382</v>
+        <v>870782886967627900000</v>
       </c>
     </row>
     <row r="102">

</xml_diff>

<commit_message>
add shadow or role, make it work on android
</commit_message>
<xml_diff>
--- a/excelToJson/Value.xlsx
+++ b/excelToJson/Value.xlsx
@@ -1160,7 +1160,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="1">
-        <v>35717</v>
+        <v>19134</v>
       </c>
       <c r="C34" s="1">
         <v>600</v>
@@ -1198,7 +1198,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>52080</v>
+        <v>20832</v>
       </c>
       <c r="C36" s="1">
         <v>660</v>
@@ -1217,7 +1217,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="1">
-        <v>39284</v>
+        <v>31427</v>
       </c>
       <c r="C37" s="1">
         <v>678</v>
@@ -1236,7 +1236,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="1">
-        <v>39573</v>
+        <v>34296</v>
       </c>
       <c r="C38" s="1">
         <v>702</v>
@@ -1255,7 +1255,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="1">
-        <v>39852</v>
+        <v>37195</v>
       </c>
       <c r="C39" s="1">
         <v>726</v>
@@ -1274,7 +1274,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>40056</v>
+        <v>37385</v>
       </c>
       <c r="C40" s="1">
         <v>744</v>
@@ -1293,7 +1293,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>80897</v>
+        <v>45842</v>
       </c>
       <c r="C41" s="1">
         <v>780</v>
@@ -1312,7 +1312,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="1">
-        <v>81647</v>
+        <v>32659</v>
       </c>
       <c r="C42" s="1">
         <v>816</v>
@@ -1331,7 +1331,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="1">
-        <v>82365</v>
+        <v>38437</v>
       </c>
       <c r="C43" s="1">
         <v>852</v>
@@ -1350,7 +1350,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="1">
-        <v>83052</v>
+        <v>41526</v>
       </c>
       <c r="C44" s="1">
         <v>887</v>
@@ -1369,7 +1369,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="1">
-        <v>83713</v>
+        <v>30694</v>
       </c>
       <c r="C45" s="1">
         <v>924</v>
@@ -1388,7 +1388,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="1">
-        <v>112464</v>
+        <v>47797</v>
       </c>
       <c r="C46" s="1">
         <v>959</v>
@@ -1407,7 +1407,7 @@
         <v>46</v>
       </c>
       <c r="B47" s="1">
-        <v>84960</v>
+        <v>39648</v>
       </c>
       <c r="C47" s="1">
         <v>996</v>
@@ -1426,7 +1426,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="1">
-        <v>85550</v>
+        <v>31368</v>
       </c>
       <c r="C48" s="1">
         <v>1032</v>
@@ -1445,7 +1445,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>86120</v>
+        <v>45930</v>
       </c>
       <c r="C49" s="1">
         <v>1068</v>
@@ -1464,7 +1464,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>86671</v>
+        <v>34668</v>
       </c>
       <c r="C50" s="1">
         <v>1104</v>
@@ -1483,7 +1483,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="1">
-        <v>116272</v>
+        <v>58136</v>
       </c>
       <c r="C51" s="1">
         <v>1140</v>
@@ -1502,7 +1502,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="1">
-        <v>87806</v>
+        <v>35122</v>
       </c>
       <c r="C52" s="1">
         <v>1182</v>
@@ -1521,7 +1521,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="1">
-        <v>88386</v>
+        <v>47139</v>
       </c>
       <c r="C53" s="1">
         <v>1223</v>
@@ -1540,7 +1540,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="1">
-        <v>88947</v>
+        <v>41508</v>
       </c>
       <c r="C54" s="1">
         <v>1266</v>
@@ -1559,7 +1559,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="1">
-        <v>89489</v>
+        <v>59659</v>
       </c>
       <c r="C55" s="1">
         <v>1307</v>
@@ -1578,7 +1578,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>120019</v>
+        <v>60009</v>
       </c>
       <c r="C56" s="1">
         <v>1350</v>
@@ -1597,7 +1597,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="1">
-        <v>90523</v>
+        <v>48279</v>
       </c>
       <c r="C57" s="1">
         <v>1391</v>
@@ -1616,7 +1616,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="1">
-        <v>91017</v>
+        <v>48542</v>
       </c>
       <c r="C58" s="1">
         <v>1434</v>
@@ -1635,7 +1635,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="1">
-        <v>91497</v>
+        <v>60998</v>
       </c>
       <c r="C59" s="1">
         <v>1476</v>
@@ -1654,7 +1654,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="1">
-        <v>91964</v>
+        <v>55178</v>
       </c>
       <c r="C60" s="1">
         <v>1518</v>
@@ -1673,7 +1673,7 @@
         <v>60</v>
       </c>
       <c r="B61" s="1">
-        <v>184835</v>
+        <v>73934</v>
       </c>
       <c r="C61" s="1">
         <v>1560</v>
@@ -1692,7 +1692,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="1">
-        <v>185842</v>
+        <v>49558</v>
       </c>
       <c r="C62" s="1">
         <v>1607</v>
@@ -1711,7 +1711,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1">
-        <v>186820</v>
+        <v>62273</v>
       </c>
       <c r="C63" s="1">
         <v>1655</v>
@@ -1730,7 +1730,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>187770</v>
+        <v>56331</v>
       </c>
       <c r="C64" s="1">
         <v>1704</v>
@@ -1749,7 +1749,7 @@
         <v>64</v>
       </c>
       <c r="B65" s="1">
-        <v>188693</v>
+        <v>81767</v>
       </c>
       <c r="C65" s="1">
         <v>1752</v>
@@ -1768,7 +1768,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="1">
-        <v>252789</v>
+        <v>56877</v>
       </c>
       <c r="C66" s="1">
         <v>1800</v>
@@ -1787,7 +1787,7 @@
         <v>66</v>
       </c>
       <c r="B67" s="1">
-        <v>190466</v>
+        <v>69837</v>
       </c>
       <c r="C67" s="1">
         <v>1848</v>
@@ -1806,7 +1806,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
-        <v>191319</v>
+        <v>82904</v>
       </c>
       <c r="C68" s="1">
         <v>1896</v>
@@ -1825,7 +1825,7 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
-        <v>192150</v>
+        <v>89670</v>
       </c>
       <c r="C69" s="1">
         <v>1943</v>
@@ -1844,7 +1844,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="1">
-        <v>192960</v>
+        <v>64320</v>
       </c>
       <c r="C70" s="1">
         <v>1991</v>
@@ -1863,7 +1863,7 @@
         <v>70</v>
       </c>
       <c r="B71" s="1">
-        <v>322920</v>
+        <v>103334</v>
       </c>
       <c r="C71" s="1">
         <v>2040</v>
@@ -1882,7 +1882,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="1">
-        <v>194620</v>
+        <v>64873</v>
       </c>
       <c r="C72" s="1">
         <v>2094</v>
@@ -1901,7 +1901,7 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
-        <v>195467</v>
+        <v>65155</v>
       </c>
       <c r="C73" s="1">
         <v>2148</v>
@@ -1920,7 +1920,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
-        <v>196292</v>
+        <v>91603</v>
       </c>
       <c r="C74" s="1">
         <v>2202</v>
@@ -1939,7 +1939,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="1">
-        <v>197097</v>
+        <v>98548</v>
       </c>
       <c r="C75" s="1">
         <v>2256</v>
@@ -1958,7 +1958,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="1">
-        <v>263845</v>
+        <v>72557</v>
       </c>
       <c r="C76" s="1">
         <v>2310</v>
@@ -1977,7 +1977,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="1">
-        <v>198652</v>
+        <v>92704</v>
       </c>
       <c r="C77" s="1">
         <v>2364</v>
@@ -1996,7 +1996,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <v>199402</v>
+        <v>106348</v>
       </c>
       <c r="C78" s="1">
         <v>2418</v>
@@ -2015,7 +2015,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <v>200136</v>
+        <v>113410</v>
       </c>
       <c r="C79" s="1">
         <v>2472</v>
@@ -2034,7 +2034,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="1">
-        <v>200855</v>
+        <v>107122</v>
       </c>
       <c r="C80" s="1">
         <v>2525</v>
@@ -2053,7 +2053,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="1">
-        <v>335930</v>
+        <v>161246</v>
       </c>
       <c r="C81" s="1">
         <v>2579</v>
@@ -2072,7 +2072,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="1">
-        <v>202322</v>
+        <v>94417</v>
       </c>
       <c r="C82" s="1">
         <v>2640</v>
@@ -2091,7 +2091,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="1">
-        <v>203069</v>
+        <v>94765</v>
       </c>
       <c r="C83" s="1">
         <v>2700</v>
@@ -2110,7 +2110,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="1">
-        <v>203800</v>
+        <v>135866</v>
       </c>
       <c r="C84" s="1">
         <v>2760</v>
@@ -2129,7 +2129,7 @@
         <v>84</v>
       </c>
       <c r="B85" s="1">
-        <v>204514</v>
+        <v>149977</v>
       </c>
       <c r="C85" s="1">
         <v>2819</v>
@@ -2148,7 +2148,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="1">
-        <v>273619</v>
+        <v>157331</v>
       </c>
       <c r="C86" s="1">
         <v>2880</v>
@@ -2167,7 +2167,7 @@
         <v>86</v>
       </c>
       <c r="B87" s="1">
-        <v>205900</v>
+        <v>123540</v>
       </c>
       <c r="C87" s="1">
         <v>2940</v>
@@ -2186,7 +2186,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="1">
-        <v>206571</v>
+        <v>137714</v>
       </c>
       <c r="C88" s="1">
         <v>3000</v>
@@ -2205,7 +2205,7 @@
         <v>88</v>
       </c>
       <c r="B89" s="1">
-        <v>207229</v>
+        <v>165783</v>
       </c>
       <c r="C89" s="1">
         <v>3060</v>
@@ -2224,7 +2224,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="1">
-        <v>207295</v>
+        <v>165836</v>
       </c>
       <c r="C90" s="1">
         <v>3066</v>
@@ -2243,7 +2243,7 @@
         <v>90</v>
       </c>
       <c r="B91" s="1">
-        <v>415878</v>
+        <v>188531</v>
       </c>
       <c r="C91" s="1">
         <v>3126</v>
@@ -2262,7 +2262,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="1">
-        <v>417267</v>
+        <v>83453</v>
       </c>
       <c r="C92" s="1">
         <v>3192</v>
@@ -2281,7 +2281,7 @@
         <v>92</v>
       </c>
       <c r="B93" s="1">
-        <v>418627</v>
+        <v>111634</v>
       </c>
       <c r="C93" s="1">
         <v>3258</v>
@@ -2300,7 +2300,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="1">
-        <v>419961</v>
+        <v>193182</v>
       </c>
       <c r="C94" s="1">
         <v>3324</v>
@@ -2319,7 +2319,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="1">
-        <v>421268</v>
+        <v>196591</v>
       </c>
       <c r="C95" s="1">
         <v>3390</v>
@@ -2338,7 +2338,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="1">
-        <v>563400</v>
+        <v>169020</v>
       </c>
       <c r="C96" s="1">
         <v>3456</v>
@@ -2357,7 +2357,7 @@
         <v>96</v>
       </c>
       <c r="B97" s="1">
-        <v>423807</v>
+        <v>169523</v>
       </c>
       <c r="C97" s="1">
         <v>3522</v>
@@ -2376,7 +2376,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="1">
-        <v>425041</v>
+        <v>175684</v>
       </c>
       <c r="C98" s="1">
         <v>3587</v>
@@ -2395,7 +2395,7 @@
         <v>98</v>
       </c>
       <c r="B99" s="1">
-        <v>426253</v>
+        <v>198918</v>
       </c>
       <c r="C99" s="1">
         <v>3654</v>
@@ -2414,7 +2414,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="1">
-        <v>427443</v>
+        <v>170977</v>
       </c>
       <c r="C100" s="1">
         <v>3720</v>
@@ -2433,7 +2433,7 @@
         <v>100</v>
       </c>
       <c r="B101" s="1">
-        <v>857225</v>
+        <v>194304</v>
       </c>
       <c r="C101" s="1">
         <v>3786</v>

</xml_diff>